<commit_message>
fixed up linkage? checking now
</commit_message>
<xml_diff>
--- a/data/case2_AC.xlsx
+++ b/data/case2_AC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samho\Desktop\PhD\DC OPF\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC2AF4F-2157-4499-B68B-07D7081A2EF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{177EF143-B33D-4E00-97C8-B020181DD546}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="500" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="22620" windowHeight="13500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="hvdc" sheetId="12" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="74">
   <si>
     <t>name</t>
   </si>
@@ -258,9 +258,6 @@
   </si>
   <si>
     <t>baseMVA</t>
-  </si>
-  <si>
-    <t>marginal_cost</t>
   </si>
   <si>
     <t>Test</t>
@@ -650,15 +647,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2377B432-B755-4411-A970-729F4FF71B71}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -702,15 +699,21 @@
         <v>2</v>
       </c>
       <c r="O1" t="s">
+        <v>62</v>
+      </c>
+      <c r="P1" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
         <v>71</v>
-      </c>
-      <c r="B2" t="s">
-        <v>72</v>
       </c>
       <c r="C2">
         <v>2</v>
@@ -746,9 +749,15 @@
         <v>1E-4</v>
       </c>
       <c r="N2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
         <v>0</v>
       </c>
     </row>
@@ -761,8 +770,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:W2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1231,7 +1240,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" t="s">
         <v>10</v>

</xml_diff>